<commit_message>
Epolicy Details and Customer Details POM
</commit_message>
<xml_diff>
--- a/Exide_POM/Resources/data/data.xlsx
+++ b/Exide_POM/Resources/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14475" windowHeight="4095" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11340" windowHeight="4095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Exide" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O20"/>
+  <oleSize ref="A1:G12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -25,34 +25,28 @@
     <t>password</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>BrowserType</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>https://host19.exidelife.in/sprint2</t>
-  </si>
-  <si>
     <t>DTDATAENTRYOPR1</t>
   </si>
   <si>
     <t>exide@1234</t>
   </si>
   <si>
-    <t>ProductNameList</t>
-  </si>
-  <si>
     <t>T20-Exide Life Smart Term - Classic RP</t>
   </si>
   <si>
-    <t>ProposalFormNumber</t>
-  </si>
-  <si>
     <t>LN000001</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>proposalNo</t>
+  </si>
+  <si>
+    <t>advisorCode</t>
+  </si>
+  <si>
+    <t>accountNum</t>
   </si>
 </sst>
 </file>
@@ -121,12 +115,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,66 +426,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:4"/>
+    <row r="4" spans="1:4"/>
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="8" spans="1:2">
+    <row r="6" spans="1:4"/>
+    <row r="7" spans="1:4"/>
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1">
+    <row r="9" spans="1:4" s="1" customFormat="1">
       <c r="B9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -497,32 +482,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>60000086</v>
+      </c>
+      <c r="D2">
+        <v>1111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>